<commit_message>
residue runs being incorporated into forest_rothc, still not working though
</commit_message>
<xml_diff>
--- a/data/forest/forest_baseline_rothc_scenarios.xlsx
+++ b/data/forest/forest_baseline_rothc_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/forest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{85B62768-A828-40EF-AF07-3F9385C00B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FFC0DF3-B8B6-45CE-9AFC-F3C7C312F93E}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{85B62768-A828-40EF-AF07-3F9385C00B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16EF4BBC-8C57-4556-B22F-5328474C9451}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5A1AC2C3-5480-416B-8642-6AF824DA0643}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>lu_fp</t>
   </si>
@@ -59,9 +59,6 @@
     <t>age_fp</t>
   </si>
   <si>
-    <t>"../LEAFs/ SOC/rasters"</t>
-  </si>
-  <si>
     <t>../data/land_use/lu_Broadleaf_Deciduous_Boreal_dry.tif</t>
   </si>
   <si>
@@ -186,6 +183,12 @@
   </si>
   <si>
     <t>../data/forest/age/Needleleaf_Evergreen_Warm_temperate_dry_age.tif</t>
+  </si>
+  <si>
+    <t>../LEAFs/SOC/rasters</t>
+  </si>
+  <si>
+    <t>residue_runs</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5062A9D1-CDE3-400F-BB53-28D0D9BF758E}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,7 +1082,7 @@
     <col min="7" max="7" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1104,395 +1107,443 @@
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
       </c>
       <c r="D10">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12">
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" t="s">
         <v>50</v>
       </c>
-      <c r="G16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" t="s">
-        <v>8</v>
+      <c r="I16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed forest residue random calculations draw. running all scenarios
</commit_message>
<xml_diff>
--- a/data/forest/forest_baseline_rothc_scenarios.xlsx
+++ b/data/forest/forest_baseline_rothc_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/forest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{85B62768-A828-40EF-AF07-3F9385C00B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16EF4BBC-8C57-4556-B22F-5328474C9451}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{85B62768-A828-40EF-AF07-3F9385C00B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF7AF405-3A15-4668-9306-8896C37EE1B9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5A1AC2C3-5480-416B-8642-6AF824DA0643}"/>
   </bookViews>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5062A9D1-CDE3-400F-BB53-28D0D9BF758E}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I2:I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,13 +1113,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>14</v>
@@ -1128,7 +1128,7 @@
         <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
@@ -1137,18 +1137,18 @@
         <v>50</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>14</v>
@@ -1157,7 +1157,7 @@
         <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -1166,7 +1166,7 @@
         <v>50</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1195,7 +1195,7 @@
         <v>50</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1224,7 +1224,7 @@
         <v>50</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1253,7 +1253,7 @@
         <v>50</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1282,18 +1282,18 @@
         <v>50</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>14</v>
@@ -1302,7 +1302,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>33</v>
@@ -1311,18 +1311,18 @@
         <v>50</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>14</v>
@@ -1331,7 +1331,7 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
@@ -1340,7 +1340,7 @@
         <v>50</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1369,7 +1369,7 @@
         <v>50</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>50</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1427,7 +1427,7 @@
         <v>50</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1456,7 +1456,7 @@
         <v>50</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1485,7 +1485,7 @@
         <v>50</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,7 +1514,7 @@
         <v>50</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>50</v>
       </c>
       <c r="I16">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>